<commit_message>
feat: pursuing the intuition for regularisation
- nearing to the final values to alpha and lambda.
- 3 more submit can conclude the values
</commit_message>
<xml_diff>
--- a/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
+++ b/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padmaraj.bhat\OneDrive - Accenture\Git\GitHub\Kaggle Competetion\House Prices- Advance Regression Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F1C41CEF-0391-45BE-853D-14FFB9667B15}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{02453C2E-9960-4815-86FA-954C37ED71A1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4110" firstSheet="8" activeTab="11" xr2:uid="{E502ACE3-46F0-4C50-944D-DCCB88A6A330}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="33">
   <si>
     <t>validation_score</t>
   </si>
@@ -138,6 +138,16 @@
   <si>
     <t>alpha = .5, lambda = 0</t>
   </si>
+  <si>
+    <t>alpha = 1, lambda = 0</t>
+  </si>
+  <si>
+    <t>alpha = 1, lambda = .5</t>
+  </si>
+  <si>
+    <t>This will fix the lambda position
+This will also give intution of alpha &gt; 1</t>
+  </si>
 </sst>
 </file>
 
@@ -178,12 +188,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -29801,10 +29814,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE418E7-1197-4C14-B4E7-FDD6E039CCEC}">
-  <dimension ref="A5:O63"/>
+  <dimension ref="A5:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="O66" sqref="O66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30824,15 +30837,64 @@
       <c r="B61" t="s">
         <v>27</v>
       </c>
+      <c r="G61">
+        <v>6</v>
+      </c>
+      <c r="H61">
+        <v>100</v>
+      </c>
+      <c r="I61">
+        <v>0.25</v>
+      </c>
+      <c r="N61">
+        <v>0.14405999999999999</v>
+      </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>28</v>
       </c>
+      <c r="G62">
+        <v>6</v>
+      </c>
+      <c r="H62">
+        <v>100</v>
+      </c>
+      <c r="I62">
+        <v>0.25</v>
+      </c>
+      <c r="N62">
+        <v>0.14230999999999999</v>
+      </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>29</v>
+      </c>
+      <c r="G63">
+        <v>6</v>
+      </c>
+      <c r="H63">
+        <v>100</v>
+      </c>
+      <c r="I63">
+        <v>0.25</v>
+      </c>
+      <c r="N63">
+        <v>0.13972999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: regularisation final values
- concluding the values of alpha and lambda as 0.5
</commit_message>
<xml_diff>
--- a/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
+++ b/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padmaraj.bhat\OneDrive - Accenture\Git\GitHub\Kaggle Competetion\House Prices- Advance Regression Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{02453C2E-9960-4815-86FA-954C37ED71A1}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BA5483DF-C134-46C0-9AC5-8181E219C2B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4110" firstSheet="8" activeTab="11" xr2:uid="{E502ACE3-46F0-4C50-944D-DCCB88A6A330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4110" firstSheet="8" activeTab="12" xr2:uid="{E502ACE3-46F0-4C50-944D-DCCB88A6A330}"/>
   </bookViews>
   <sheets>
     <sheet name="Without estimator" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="alphalambda1" sheetId="11" r:id="rId10"/>
     <sheet name="alphalambdagrid" sheetId="12" r:id="rId11"/>
     <sheet name="Comparison of best scores" sheetId="5" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">alpha_.5!$D$3:$J$132</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="35">
   <si>
     <t>validation_score</t>
   </si>
@@ -147,6 +148,12 @@
   <si>
     <t>This will fix the lambda position
 This will also give intution of alpha &gt; 1</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>big</t>
   </si>
 </sst>
 </file>
@@ -29816,8 +29823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE418E7-1197-4C14-B4E7-FDD6E039CCEC}">
   <dimension ref="A5:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="O66" sqref="O66"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30846,6 +30853,9 @@
       <c r="I61">
         <v>0.25</v>
       </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
       <c r="N61">
         <v>0.14405999999999999</v>
       </c>
@@ -30863,6 +30873,9 @@
       <c r="I62">
         <v>0.25</v>
       </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
       <c r="N62">
         <v>0.14230999999999999</v>
       </c>
@@ -30880,6 +30893,9 @@
       <c r="I63">
         <v>0.25</v>
       </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
       <c r="N63">
         <v>0.13972999999999999</v>
       </c>
@@ -30888,11 +30904,41 @@
       <c r="B64" t="s">
         <v>30</v>
       </c>
+      <c r="G64">
+        <v>6</v>
+      </c>
+      <c r="H64">
+        <v>100</v>
+      </c>
+      <c r="I64">
+        <v>0.25</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>0.14047000000000001</v>
+      </c>
     </row>
     <row r="65" spans="2:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>31</v>
       </c>
+      <c r="G65">
+        <v>6</v>
+      </c>
+      <c r="H65">
+        <v>100</v>
+      </c>
+      <c r="I65">
+        <v>0.25</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="N65" s="4">
+        <v>0.14396</v>
+      </c>
       <c r="O65" s="4" t="s">
         <v>32</v>
       </c>
@@ -30900,6 +30946,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4958B2F9-4C94-434D-BF59-730962F1114A}">
+  <dimension ref="C3:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.14435000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.13972999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.14405999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.13913</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.14047000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.14396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
docs: target variable / GrLivArea
- target variable transformation result for SalePrice / GrLivArea
</commit_message>
<xml_diff>
--- a/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
+++ b/House Prices- Advanced Regression Techniques/ML/GridSearchResultsFromKaggle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padmaraj.bhat\OneDrive - Accenture\Git\GitHub\Kaggle Competetion\House Prices- Advance Regression Techniques\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/padmaraj_bhat_accenture_com/Documents/Git/GitHub/Kaggle Competetion/House Prices- Advance Regression Techniques/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BA5483DF-C134-46C0-9AC5-8181E219C2B6}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="10_ncr:100000_{28F5228C-9FC8-4E39-B27D-CA503DA6A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2EDD1618-58F1-42E7-96A3-EFF208E4465C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4110" firstSheet="8" activeTab="12" xr2:uid="{E502ACE3-46F0-4C50-944D-DCCB88A6A330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4110" firstSheet="11" activeTab="13" xr2:uid="{E502ACE3-46F0-4C50-944D-DCCB88A6A330}"/>
   </bookViews>
   <sheets>
     <sheet name="Without estimator" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="alphalambda1" sheetId="11" r:id="rId10"/>
     <sheet name="alphalambdagrid" sheetId="12" r:id="rId11"/>
     <sheet name="Comparison of best scores" sheetId="5" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
+    <sheet name="Regularization exp" sheetId="13" r:id="rId13"/>
+    <sheet name="TargetTrans 1" sheetId="14" r:id="rId14"/>
+    <sheet name="TargetTrans2" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">alpha_.5!$D$3:$J$132</definedName>
@@ -34,6 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">alphalambdagrid!$E$4:$M$104</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">alphalambdaminmax!$D$4:$J$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">minmaxagain!$E$5:$K$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">TargetTrans2!$C$5:$I$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'transformed rmsle - target'!$C$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'with estimator'!$D$2:$J$1282</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Without estimator'!$C$3:$J$899</definedName>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="38">
   <si>
     <t>validation_score</t>
   </si>
@@ -154,6 +157,15 @@
   </si>
   <si>
     <t>big</t>
+  </si>
+  <si>
+    <t>target / liv area</t>
+  </si>
+  <si>
+    <t>log(target/grlivarea)</t>
+  </si>
+  <si>
+    <t>Kaggle Score</t>
   </si>
 </sst>
 </file>
@@ -29823,8 +29835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE418E7-1197-4C14-B4E7-FDD6E039CCEC}">
   <dimension ref="A5:O65"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30953,8 +30965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4958B2F9-4C94-434D-BF59-730962F1114A}">
   <dimension ref="C3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30966,6 +30978,9 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C4">
@@ -31054,6 +31069,4418 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A5DEAB-988D-4848-AD8E-E603EF1C0517}">
+  <dimension ref="D2:J81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>5.4548754571017898E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.144820275592943</v>
+      </c>
+      <c r="F5">
+        <v>0.136749211288926</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>7.1911992256777302E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.14379293899481599</v>
+      </c>
+      <c r="F6">
+        <v>0.13779100460461699</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>7.3091547806251697E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.142897849401006</v>
+      </c>
+      <c r="F7">
+        <v>0.13790856602996701</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>3.8625986021367097E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.14594485779341099</v>
+      </c>
+      <c r="F8">
+        <v>0.13797876242805401</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>5.6211513319048799E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.14353332654971401</v>
+      </c>
+      <c r="F9">
+        <v>0.13813043050634299</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>0.75</v>
+      </c>
+      <c r="J9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>5.4042389965850098E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.144853874936508</v>
+      </c>
+      <c r="F10">
+        <v>0.13888831262376999</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>0.75</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>5.5337556341240601E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.143810092892311</v>
+      </c>
+      <c r="F11">
+        <v>0.13897623030487299</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>0.75</v>
+      </c>
+      <c r="J11">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>7.8906250332581598E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.143864377108705</v>
+      </c>
+      <c r="F12">
+        <v>0.139233994694758</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>7.3385259676137807E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.14371433859809701</v>
+      </c>
+      <c r="F13">
+        <v>0.13935162116566099</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>0.75</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>5.37622189396018E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.14431278306599801</v>
+      </c>
+      <c r="F14">
+        <v>0.13950767798069</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>3.8772400727886597E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.14595355161402901</v>
+      </c>
+      <c r="F15">
+        <v>0.13965736471264201</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>0.75</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>5.5089202377281703E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.14381422774526201</v>
+      </c>
+      <c r="F16">
+        <v>0.13994338089551001</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>7.6930887180720997E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.143272748826519</v>
+      </c>
+      <c r="F17">
+        <v>0.14003951951701299</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>0.75</v>
+      </c>
+      <c r="J17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>5.4657541532154602E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.14459376519176001</v>
+      </c>
+      <c r="F18">
+        <v>0.140062729959299</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>0.5</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>6.2990188660679E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.14458974697801399</v>
+      </c>
+      <c r="F19">
+        <v>0.140106775875878</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>0.25</v>
+      </c>
+      <c r="J19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>5.5494560007144103E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.14388741503302999</v>
+      </c>
+      <c r="F20">
+        <v>0.14011900790888299</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>0.5</v>
+      </c>
+      <c r="J20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>7.6715119398345494E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.14305187975418401</v>
+      </c>
+      <c r="F21">
+        <v>0.140250197406906</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>7.3930564069416296E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.14396387598010199</v>
+      </c>
+      <c r="F22">
+        <v>0.14031005364490401</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>0.75</v>
+      </c>
+      <c r="J22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <v>4.03986534667653E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.14549291045475499</v>
+      </c>
+      <c r="F23">
+        <v>0.14059006980165201</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <v>4.2533187872761197E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.14473203937564999</v>
+      </c>
+      <c r="F24">
+        <v>0.140749720515807</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <v>0.75</v>
+      </c>
+      <c r="J24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>7.8964749047673297E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.14180827766998499</v>
+      </c>
+      <c r="F25">
+        <v>0.14085987955818399</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>100</v>
+      </c>
+      <c r="I25">
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>7.6075198717885997E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.143898202797585</v>
+      </c>
+      <c r="F26">
+        <v>0.140993506077294</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26">
+        <v>0.5</v>
+      </c>
+      <c r="J26">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>3.9080107406913603E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.14591264905616999</v>
+      </c>
+      <c r="F27">
+        <v>0.14103106670497301</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
+      <c r="I27">
+        <v>0.75</v>
+      </c>
+      <c r="J27">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>4.5094409343118903E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.14539096413747599</v>
+      </c>
+      <c r="F28">
+        <v>0.141099478659726</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>5.9134490933441301E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.142231124724185</v>
+      </c>
+      <c r="F29">
+        <v>0.14113298000503</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>100</v>
+      </c>
+      <c r="I29">
+        <v>0.75</v>
+      </c>
+      <c r="J29">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>5.8998970281750697E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.14428476207138899</v>
+      </c>
+      <c r="F30">
+        <v>0.14115522589653301</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>100</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>4.7851600507967003E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.145011749472016</v>
+      </c>
+      <c r="F31">
+        <v>0.141338479482813</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>100</v>
+      </c>
+      <c r="I31">
+        <v>0.5</v>
+      </c>
+      <c r="J31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>7.8444975810395196E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.143627856523838</v>
+      </c>
+      <c r="F32">
+        <v>0.14148386350700601</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>3.9636606104035702E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.14494753412293901</v>
+      </c>
+      <c r="F33">
+        <v>0.14151293788243899</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <v>100</v>
+      </c>
+      <c r="I33">
+        <v>0.75</v>
+      </c>
+      <c r="J33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>2.9574059721304499E-2</v>
+      </c>
+      <c r="E34">
+        <v>0.145998903467953</v>
+      </c>
+      <c r="F34">
+        <v>0.14160285192813499</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+      <c r="I34">
+        <v>0.5</v>
+      </c>
+      <c r="J34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>6.4117810724172997E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.144254490636922</v>
+      </c>
+      <c r="F35">
+        <v>0.141624774483881</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>100</v>
+      </c>
+      <c r="I35">
+        <v>0.5</v>
+      </c>
+      <c r="J35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>2.7999486392233298E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.146093642650866</v>
+      </c>
+      <c r="F36">
+        <v>0.141709723172004</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <v>100</v>
+      </c>
+      <c r="I36">
+        <v>0.75</v>
+      </c>
+      <c r="J36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>3.08661459161239E-2</v>
+      </c>
+      <c r="E37">
+        <v>0.145411940498862</v>
+      </c>
+      <c r="F37">
+        <v>0.141741880823363</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
+      </c>
+      <c r="I37">
+        <v>0.75</v>
+      </c>
+      <c r="J37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>7.9172793200306693E-2</v>
+      </c>
+      <c r="E38">
+        <v>0.14466145201642999</v>
+      </c>
+      <c r="F38">
+        <v>0.14177054262946401</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
+      <c r="I38">
+        <v>0.25</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>7.4367557900059694E-2</v>
+      </c>
+      <c r="E39">
+        <v>0.14384887135478699</v>
+      </c>
+      <c r="F39">
+        <v>0.14183474269000601</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>100</v>
+      </c>
+      <c r="I39">
+        <v>0.5</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>2.84596400716783E-2</v>
+      </c>
+      <c r="E40">
+        <v>0.14782351763776699</v>
+      </c>
+      <c r="F40">
+        <v>0.14187995466110501</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
+      </c>
+      <c r="I40">
+        <v>0.75</v>
+      </c>
+      <c r="J40">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>8.4092033389694107E-2</v>
+      </c>
+      <c r="E41">
+        <v>0.14311683047464299</v>
+      </c>
+      <c r="F41">
+        <v>0.14189998701913201</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>100</v>
+      </c>
+      <c r="I41">
+        <v>0.25</v>
+      </c>
+      <c r="J41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>4.2498208712520698E-2</v>
+      </c>
+      <c r="E42">
+        <v>0.14534346507687801</v>
+      </c>
+      <c r="F42">
+        <v>0.14196124165475399</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+      <c r="I42">
+        <v>0.5</v>
+      </c>
+      <c r="J42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>7.90616794151974E-2</v>
+      </c>
+      <c r="E43">
+        <v>0.143294619441518</v>
+      </c>
+      <c r="F43">
+        <v>0.14199601953748101</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <v>100</v>
+      </c>
+      <c r="I43">
+        <v>0.75</v>
+      </c>
+      <c r="J43">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>5.9665125859145997E-2</v>
+      </c>
+      <c r="E44">
+        <v>0.14548768593693701</v>
+      </c>
+      <c r="F44">
+        <v>0.142052842585591</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44">
+        <v>100</v>
+      </c>
+      <c r="I44">
+        <v>0.25</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>3.7582786395343001E-2</v>
+      </c>
+      <c r="E45">
+        <v>0.14672207069477999</v>
+      </c>
+      <c r="F45">
+        <v>0.14207354429727401</v>
+      </c>
+      <c r="G45">
+        <v>6</v>
+      </c>
+      <c r="H45">
+        <v>100</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>2.9688762132354399E-2</v>
+      </c>
+      <c r="E46">
+        <v>0.146174546741619</v>
+      </c>
+      <c r="F46">
+        <v>0.14216420531681401</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46">
+        <v>100</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>3.7456656647000999E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.14875770038600999</v>
+      </c>
+      <c r="F47">
+        <v>0.14224472054533399</v>
+      </c>
+      <c r="G47">
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <v>100</v>
+      </c>
+      <c r="I47">
+        <v>0.25</v>
+      </c>
+      <c r="J47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>3.9728689003055498E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.14596919333043801</v>
+      </c>
+      <c r="F48">
+        <v>0.142262493066655</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <v>100</v>
+      </c>
+      <c r="I48">
+        <v>0.5</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>5.7678248100613498E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.14406362123383001</v>
+      </c>
+      <c r="F49">
+        <v>0.14226986504319999</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>100</v>
+      </c>
+      <c r="I49">
+        <v>0.5</v>
+      </c>
+      <c r="J49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <v>2.6811223860746299E-2</v>
+      </c>
+      <c r="E50">
+        <v>0.14758372839689299</v>
+      </c>
+      <c r="F50">
+        <v>0.14252442777440499</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
+        <v>100</v>
+      </c>
+      <c r="I50">
+        <v>0.75</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D51">
+        <v>9.30671950296557E-2</v>
+      </c>
+      <c r="E51">
+        <v>0.144697616335349</v>
+      </c>
+      <c r="F51">
+        <v>0.14260116319103</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>100</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D52">
+        <v>4.4138439767757498E-2</v>
+      </c>
+      <c r="E52">
+        <v>0.14686381306214499</v>
+      </c>
+      <c r="F52">
+        <v>0.14265666307473801</v>
+      </c>
+      <c r="G52">
+        <v>6</v>
+      </c>
+      <c r="H52">
+        <v>100</v>
+      </c>
+      <c r="I52">
+        <v>0.25</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D53">
+        <v>2.6863738765542901E-2</v>
+      </c>
+      <c r="E53">
+        <v>0.147110634271407</v>
+      </c>
+      <c r="F53">
+        <v>0.14277763763182499</v>
+      </c>
+      <c r="G53">
+        <v>7</v>
+      </c>
+      <c r="H53">
+        <v>100</v>
+      </c>
+      <c r="I53">
+        <v>0.5</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D54">
+        <v>5.7952255000283399E-2</v>
+      </c>
+      <c r="E54">
+        <v>0.14525152239228101</v>
+      </c>
+      <c r="F54">
+        <v>0.14287951865478801</v>
+      </c>
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54">
+        <v>100</v>
+      </c>
+      <c r="I54">
+        <v>0.25</v>
+      </c>
+      <c r="J54">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D55">
+        <v>4.0729455610341199E-2</v>
+      </c>
+      <c r="E55">
+        <v>0.145249436821453</v>
+      </c>
+      <c r="F55">
+        <v>0.14291940904627901</v>
+      </c>
+      <c r="G55">
+        <v>6</v>
+      </c>
+      <c r="H55">
+        <v>100</v>
+      </c>
+      <c r="I55">
+        <v>0.5</v>
+      </c>
+      <c r="J55">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D56">
+        <v>9.4525454096740097E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.14502937314563399</v>
+      </c>
+      <c r="F56">
+        <v>0.143187702568152</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>100</v>
+      </c>
+      <c r="I56">
+        <v>0.75</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D57">
+        <v>9.2750405613828399E-2</v>
+      </c>
+      <c r="E57">
+        <v>0.144515720797462</v>
+      </c>
+      <c r="F57">
+        <v>0.143248470752045</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <v>100</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D58">
+        <v>4.7752058323928398E-2</v>
+      </c>
+      <c r="E58">
+        <v>0.14723179821040699</v>
+      </c>
+      <c r="F58">
+        <v>0.14334759707599101</v>
+      </c>
+      <c r="G58">
+        <v>6</v>
+      </c>
+      <c r="H58">
+        <v>100</v>
+      </c>
+      <c r="I58">
+        <v>0.25</v>
+      </c>
+      <c r="J58">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D59">
+        <v>3.1794926720318702E-2</v>
+      </c>
+      <c r="E59">
+        <v>0.14801149050100301</v>
+      </c>
+      <c r="F59">
+        <v>0.143536213317284</v>
+      </c>
+      <c r="G59">
+        <v>7</v>
+      </c>
+      <c r="H59">
+        <v>100</v>
+      </c>
+      <c r="I59">
+        <v>0.25</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D60">
+        <v>6.5140247442255703E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.14390741486289799</v>
+      </c>
+      <c r="F60">
+        <v>0.14366811929129999</v>
+      </c>
+      <c r="G60">
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>100</v>
+      </c>
+      <c r="I60">
+        <v>0.25</v>
+      </c>
+      <c r="J60">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D61">
+        <v>8.2065369704757002E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.14330545826992999</v>
+      </c>
+      <c r="F61">
+        <v>0.14388761688785201</v>
+      </c>
+      <c r="G61">
+        <v>4</v>
+      </c>
+      <c r="H61">
+        <v>100</v>
+      </c>
+      <c r="I61">
+        <v>0.5</v>
+      </c>
+      <c r="J61">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="62" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D62">
+        <v>9.5334387809374005E-2</v>
+      </c>
+      <c r="E62">
+        <v>0.14478954060951699</v>
+      </c>
+      <c r="F62">
+        <v>0.14399934262578301</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>100</v>
+      </c>
+      <c r="I62">
+        <v>0.75</v>
+      </c>
+      <c r="J62">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D63">
+        <v>2.7931452288733501E-2</v>
+      </c>
+      <c r="E63">
+        <v>0.14632351869443599</v>
+      </c>
+      <c r="F63">
+        <v>0.14428213871301401</v>
+      </c>
+      <c r="G63">
+        <v>7</v>
+      </c>
+      <c r="H63">
+        <v>100</v>
+      </c>
+      <c r="I63">
+        <v>0.5</v>
+      </c>
+      <c r="J63">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D64">
+        <v>9.6799526278103107E-2</v>
+      </c>
+      <c r="E64">
+        <v>0.14533934612503599</v>
+      </c>
+      <c r="F64">
+        <v>0.144478706273166</v>
+      </c>
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="H64">
+        <v>100</v>
+      </c>
+      <c r="I64">
+        <v>0.75</v>
+      </c>
+      <c r="J64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D65">
+        <v>8.9695634736146695E-2</v>
+      </c>
+      <c r="E65">
+        <v>0.14500433813827199</v>
+      </c>
+      <c r="F65">
+        <v>0.14466391954532901</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>100</v>
+      </c>
+      <c r="I65">
+        <v>0.25</v>
+      </c>
+      <c r="J65">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D66">
+        <v>3.6409659290349103E-2</v>
+      </c>
+      <c r="E66">
+        <v>0.145852934434788</v>
+      </c>
+      <c r="F66">
+        <v>0.14466650506728401</v>
+      </c>
+      <c r="G66">
+        <v>7</v>
+      </c>
+      <c r="H66">
+        <v>100</v>
+      </c>
+      <c r="I66">
+        <v>0.5</v>
+      </c>
+      <c r="J66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="67" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D67">
+        <v>0.10041110748656901</v>
+      </c>
+      <c r="E67">
+        <v>0.14606379212988399</v>
+      </c>
+      <c r="F67">
+        <v>0.14523852550067501</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>100</v>
+      </c>
+      <c r="I67">
+        <v>0.25</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D68">
+        <v>9.7996420864849498E-2</v>
+      </c>
+      <c r="E68">
+        <v>0.14425340389809499</v>
+      </c>
+      <c r="F68">
+        <v>0.145334142176821</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>100</v>
+      </c>
+      <c r="I68">
+        <v>0.5</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D69">
+        <v>9.6119638209375302E-2</v>
+      </c>
+      <c r="E69">
+        <v>0.144703652222856</v>
+      </c>
+      <c r="F69">
+        <v>0.14566033826557101</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69">
+        <v>100</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D70">
+        <v>0.10034936223888601</v>
+      </c>
+      <c r="E70">
+        <v>0.14507977194236499</v>
+      </c>
+      <c r="F70">
+        <v>0.145764543087638</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>100</v>
+      </c>
+      <c r="I70">
+        <v>0.5</v>
+      </c>
+      <c r="J70">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D71">
+        <v>4.48065160277442E-2</v>
+      </c>
+      <c r="E71">
+        <v>0.146547532455121</v>
+      </c>
+      <c r="F71">
+        <v>0.14582467532940699</v>
+      </c>
+      <c r="G71">
+        <v>6</v>
+      </c>
+      <c r="H71">
+        <v>100</v>
+      </c>
+      <c r="I71">
+        <v>0.25</v>
+      </c>
+      <c r="J71">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D72">
+        <v>9.7707346415182403E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.14504002959333001</v>
+      </c>
+      <c r="F72">
+        <v>0.146210693825431</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>100</v>
+      </c>
+      <c r="I72">
+        <v>0.5</v>
+      </c>
+      <c r="J72">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="73" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D73">
+        <v>0.10123673069099801</v>
+      </c>
+      <c r="E73">
+        <v>0.144636494612358</v>
+      </c>
+      <c r="F73">
+        <v>0.146570473997262</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>100</v>
+      </c>
+      <c r="I73">
+        <v>0.25</v>
+      </c>
+      <c r="J73">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="74" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D74">
+        <v>3.3673849442253399E-2</v>
+      </c>
+      <c r="E74">
+        <v>0.14835729412493301</v>
+      </c>
+      <c r="F74">
+        <v>0.14701391525052701</v>
+      </c>
+      <c r="G74">
+        <v>7</v>
+      </c>
+      <c r="H74">
+        <v>100</v>
+      </c>
+      <c r="I74">
+        <v>0.25</v>
+      </c>
+      <c r="J74">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="75" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D75">
+        <v>4.6489795105927802E-2</v>
+      </c>
+      <c r="E75">
+        <v>0.14810273268039301</v>
+      </c>
+      <c r="F75">
+        <v>0.14757263809645799</v>
+      </c>
+      <c r="G75">
+        <v>7</v>
+      </c>
+      <c r="H75">
+        <v>100</v>
+      </c>
+      <c r="I75">
+        <v>0.25</v>
+      </c>
+      <c r="J75">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="76" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D76">
+        <v>9.9902195737285204E-2</v>
+      </c>
+      <c r="E76">
+        <v>0.145662755796407</v>
+      </c>
+      <c r="F76">
+        <v>0.148250510933949</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="H76">
+        <v>100</v>
+      </c>
+      <c r="I76">
+        <v>0.75</v>
+      </c>
+      <c r="J76">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="77" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D77">
+        <v>9.9227075320813096E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.145372651423302</v>
+      </c>
+      <c r="F77">
+        <v>0.14864788108615101</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77">
+        <v>100</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="78" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D78">
+        <v>0.104516350389491</v>
+      </c>
+      <c r="E78">
+        <v>0.14636672595199801</v>
+      </c>
+      <c r="F78">
+        <v>0.148825707583505</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
+      <c r="H78">
+        <v>100</v>
+      </c>
+      <c r="I78">
+        <v>0.5</v>
+      </c>
+      <c r="J78">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="79" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D79">
+        <v>0.103910978736291</v>
+      </c>
+      <c r="E79">
+        <v>0.14584939370680899</v>
+      </c>
+      <c r="F79">
+        <v>0.14897067744436199</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>100</v>
+      </c>
+      <c r="I79">
+        <v>0.25</v>
+      </c>
+      <c r="J79">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D80">
+        <v>7.4262983483640105E-2</v>
+      </c>
+      <c r="E80">
+        <v>0.14563137942724</v>
+      </c>
+      <c r="F80">
+        <v>0.14935423530904501</v>
+      </c>
+      <c r="G80">
+        <v>5</v>
+      </c>
+      <c r="H80">
+        <v>100</v>
+      </c>
+      <c r="I80">
+        <v>0.25</v>
+      </c>
+      <c r="J80">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D81">
+        <v>0.11175602371724901</v>
+      </c>
+      <c r="E81">
+        <v>0.147262347287127</v>
+      </c>
+      <c r="F81">
+        <v>0.153803016649456</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81">
+        <v>100</v>
+      </c>
+      <c r="I81">
+        <v>0.25</v>
+      </c>
+      <c r="J81">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D5:J81">
+    <sortCondition ref="F4"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7798C406-FA98-4DF6-9C78-7FBAA4E1614F}">
+  <dimension ref="C3:K115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>0.14480999999999999</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>0.14582999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>7.1248074702252598E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.142798635244375</v>
+      </c>
+      <c r="E6">
+        <v>0.13042777691013099</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>0.75</v>
+      </c>
+      <c r="I6">
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>0.14452999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>4.9418672328583997E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.144430286011517</v>
+      </c>
+      <c r="E7">
+        <v>0.131186066111282</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>0.75</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>5.5065952546256097E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.14227228940248501</v>
+      </c>
+      <c r="E8">
+        <v>0.13191177435762799</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>0.75</v>
+      </c>
+      <c r="I8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>4.9737309691696902E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.14370256374747001</v>
+      </c>
+      <c r="E9">
+        <v>0.131975342310517</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>7.3510953676715104E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.14285157588931299</v>
+      </c>
+      <c r="E10">
+        <v>0.132010621377112</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>0.75</v>
+      </c>
+      <c r="I10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>6.2212412102181397E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.14329656402020499</v>
+      </c>
+      <c r="E11">
+        <v>0.132195823796705</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0.75</v>
+      </c>
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>6.3279494419916302E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.143583971447724</v>
+      </c>
+      <c r="E12">
+        <v>0.132447083580086</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>4.5169636495339498E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.145612965121141</v>
+      </c>
+      <c r="E13">
+        <v>0.13251167987829901</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>0.75</v>
+      </c>
+      <c r="I13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>4.6358230172980297E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.14542082345627599</v>
+      </c>
+      <c r="E14">
+        <v>0.132566993043613</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>5.15885866099157E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.14447780817421199</v>
+      </c>
+      <c r="E15">
+        <v>0.13270082890635501</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>4.2405894122466002E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.146577870396389</v>
+      </c>
+      <c r="E16">
+        <v>0.13274587052254</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>6.2866032909842107E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.14343244822811499</v>
+      </c>
+      <c r="E17">
+        <v>0.133033839302411</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>0.75</v>
+      </c>
+      <c r="I17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>5.32207551499633E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.14401821165966899</v>
+      </c>
+      <c r="E18">
+        <v>0.133165347544275</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>5.4044439049603002E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.14323403646300301</v>
+      </c>
+      <c r="E19">
+        <v>0.133256498083314</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>6.15621799422588E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.14405905121283599</v>
+      </c>
+      <c r="E20">
+        <v>0.13360554776109601</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>4.6749842296240303E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.14484142340377101</v>
+      </c>
+      <c r="E21">
+        <v>0.13366274211245099</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>0.5</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>6.1877018212966199E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.14201522102592201</v>
+      </c>
+      <c r="E22">
+        <v>0.13373893441908699</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>0.75</v>
+      </c>
+      <c r="I22">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>6.0043044365592803E-2</v>
+      </c>
+      <c r="D23">
+        <v>0.142714272369248</v>
+      </c>
+      <c r="E23">
+        <v>0.133757888097077</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>5.5447738778628602E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.143837352346112</v>
+      </c>
+      <c r="E24">
+        <v>0.13406009704069199</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>4.6974964050424603E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.14488499077929701</v>
+      </c>
+      <c r="E25">
+        <v>0.13422688287816001</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>6.8073201383840098E-2</v>
+      </c>
+      <c r="D26">
+        <v>0.142265060976243</v>
+      </c>
+      <c r="E26">
+        <v>0.134242621470887</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>7.6049594524972897E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.142375747615482</v>
+      </c>
+      <c r="E27">
+        <v>0.13438435757053499</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+      <c r="H27">
+        <v>0.5</v>
+      </c>
+      <c r="I27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>5.3217961636057999E-2</v>
+      </c>
+      <c r="D28">
+        <v>0.14574087006318001</v>
+      </c>
+      <c r="E28">
+        <v>0.13462439502958701</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>4.7552974089167602E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.14402780091200201</v>
+      </c>
+      <c r="E29">
+        <v>0.134642089767083</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>0.5</v>
+      </c>
+      <c r="I29">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>7.1196566060609104E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.14341975549309999</v>
+      </c>
+      <c r="E30">
+        <v>0.13475088840924601</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>5.8420241364423801E-2</v>
+      </c>
+      <c r="D31">
+        <v>0.143001360290514</v>
+      </c>
+      <c r="E31">
+        <v>0.13507584827612501</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>100</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>6.6751234706733206E-2</v>
+      </c>
+      <c r="D32">
+        <v>0.14262735058331399</v>
+      </c>
+      <c r="E32">
+        <v>0.135202350140886</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>5.6347221915966798E-2</v>
+      </c>
+      <c r="D33">
+        <v>0.14271036879767901</v>
+      </c>
+      <c r="E33">
+        <v>0.135515210312247</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>100</v>
+      </c>
+      <c r="H33">
+        <v>0.5</v>
+      </c>
+      <c r="I33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>5.03595833383065E-2</v>
+      </c>
+      <c r="D34">
+        <v>0.14272467067533001</v>
+      </c>
+      <c r="E34">
+        <v>0.13553221937810001</v>
+      </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="G34">
+        <v>100</v>
+      </c>
+      <c r="H34">
+        <v>0.75</v>
+      </c>
+      <c r="I34">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>6.9619489624805297E-2</v>
+      </c>
+      <c r="D35">
+        <v>0.14244529893965299</v>
+      </c>
+      <c r="E35">
+        <v>0.13607691526094701</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>0.75</v>
+      </c>
+      <c r="I35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>5.58771902547621E-2</v>
+      </c>
+      <c r="D36">
+        <v>0.14383905298826699</v>
+      </c>
+      <c r="E36">
+        <v>0.13611959602038501</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>100</v>
+      </c>
+      <c r="H36">
+        <v>0.75</v>
+      </c>
+      <c r="I36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>6.8361070068934299E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.143007453947913</v>
+      </c>
+      <c r="E37">
+        <v>0.13616650069554001</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+      <c r="H37">
+        <v>0.25</v>
+      </c>
+      <c r="I37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>6.0586475917993099E-2</v>
+      </c>
+      <c r="D38">
+        <v>0.14337612599521499</v>
+      </c>
+      <c r="E38">
+        <v>0.13625442146392699</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>0.5</v>
+      </c>
+      <c r="I38">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>7.3701078604477305E-2</v>
+      </c>
+      <c r="D39">
+        <v>0.14244419937355901</v>
+      </c>
+      <c r="E39">
+        <v>0.13639290723602601</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>0.5</v>
+      </c>
+      <c r="I39">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>8.2075809229097199E-2</v>
+      </c>
+      <c r="D40">
+        <v>0.143512508018142</v>
+      </c>
+      <c r="E40">
+        <v>0.136740958268351</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>0.75</v>
+      </c>
+      <c r="I40">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>8.9141050747249206E-2</v>
+      </c>
+      <c r="D41">
+        <v>0.14288397691900201</v>
+      </c>
+      <c r="E41">
+        <v>0.136799626463811</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>0.75</v>
+      </c>
+      <c r="I41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>5.3687929703464803E-2</v>
+      </c>
+      <c r="D42">
+        <v>0.14433593301856101</v>
+      </c>
+      <c r="E42">
+        <v>0.13681467934172201</v>
+      </c>
+      <c r="F42">
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <v>100</v>
+      </c>
+      <c r="H42">
+        <v>0.75</v>
+      </c>
+      <c r="I42">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>8.4858510528274797E-2</v>
+      </c>
+      <c r="D43">
+        <v>0.14226453356164001</v>
+      </c>
+      <c r="E43">
+        <v>0.136845953075762</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>0.75</v>
+      </c>
+      <c r="I43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>5.7740583788022E-2</v>
+      </c>
+      <c r="D44">
+        <v>0.143143557904821</v>
+      </c>
+      <c r="E44">
+        <v>0.13698618878527699</v>
+      </c>
+      <c r="F44">
+        <v>7</v>
+      </c>
+      <c r="G44">
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>0.5</v>
+      </c>
+      <c r="I44">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>4.9932084975161099E-2</v>
+      </c>
+      <c r="D45">
+        <v>0.14768484192307499</v>
+      </c>
+      <c r="E45">
+        <v>0.137063359100979</v>
+      </c>
+      <c r="F45">
+        <v>7</v>
+      </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>6.4129937475176396E-2</v>
+      </c>
+      <c r="D46">
+        <v>0.142426092016919</v>
+      </c>
+      <c r="E46">
+        <v>0.13708199801426299</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+      <c r="G46">
+        <v>100</v>
+      </c>
+      <c r="H46">
+        <v>0.5</v>
+      </c>
+      <c r="I46">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>7.7667670540789602E-2</v>
+      </c>
+      <c r="D47">
+        <v>0.14256438044314201</v>
+      </c>
+      <c r="E47">
+        <v>0.13745490606313501</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+      <c r="H47">
+        <v>0.25</v>
+      </c>
+      <c r="I47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>7.4194347644089706E-2</v>
+      </c>
+      <c r="D48">
+        <v>0.14237312487564499</v>
+      </c>
+      <c r="E48">
+        <v>0.137515568551625</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>100</v>
+      </c>
+      <c r="H48">
+        <v>0.5</v>
+      </c>
+      <c r="I48">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>8.2792030794582097E-2</v>
+      </c>
+      <c r="D49">
+        <v>0.14382287802468499</v>
+      </c>
+      <c r="E49">
+        <v>0.13759596264541701</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <v>100</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <v>6.6323940553380395E-2</v>
+      </c>
+      <c r="D50">
+        <v>0.142922650521908</v>
+      </c>
+      <c r="E50">
+        <v>0.13760052146860099</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <v>100</v>
+      </c>
+      <c r="H50">
+        <v>0.5</v>
+      </c>
+      <c r="I50">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <v>5.88807012981995E-2</v>
+      </c>
+      <c r="D51">
+        <v>0.14630638505274701</v>
+      </c>
+      <c r="E51">
+        <v>0.137612379446067</v>
+      </c>
+      <c r="F51">
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>100</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>4.4687983810029301E-2</v>
+      </c>
+      <c r="D52">
+        <v>0.14777527531493601</v>
+      </c>
+      <c r="E52">
+        <v>0.13766937044303099</v>
+      </c>
+      <c r="F52">
+        <v>8</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>5.1846650517711798E-2</v>
+      </c>
+      <c r="D53">
+        <v>0.143552204318002</v>
+      </c>
+      <c r="E53">
+        <v>0.13769987270752501</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>100</v>
+      </c>
+      <c r="H53">
+        <v>0.5</v>
+      </c>
+      <c r="I53">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <v>5.1826618621187599E-2</v>
+      </c>
+      <c r="D54">
+        <v>0.14563691035496301</v>
+      </c>
+      <c r="E54">
+        <v>0.13775956740147699</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>100</v>
+      </c>
+      <c r="H54">
+        <v>0.75</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <v>7.7963361361206296E-2</v>
+      </c>
+      <c r="D55">
+        <v>0.14218554771089001</v>
+      </c>
+      <c r="E55">
+        <v>0.13779132433208499</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>100</v>
+      </c>
+      <c r="H55">
+        <v>0.75</v>
+      </c>
+      <c r="I55">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <v>7.6368696459021002E-2</v>
+      </c>
+      <c r="D56">
+        <v>0.14261702219457301</v>
+      </c>
+      <c r="E56">
+        <v>0.13793727783418999</v>
+      </c>
+      <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <v>7.2664598165924799E-2</v>
+      </c>
+      <c r="D57">
+        <v>0.14320887598780199</v>
+      </c>
+      <c r="E57">
+        <v>0.13806266405804701</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>100</v>
+      </c>
+      <c r="H57">
+        <v>0.5</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>4.3466585345451399E-2</v>
+      </c>
+      <c r="D58">
+        <v>0.148570522156551</v>
+      </c>
+      <c r="E58">
+        <v>0.13825163828270601</v>
+      </c>
+      <c r="F58">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>100</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>8.72130508347988E-2</v>
+      </c>
+      <c r="D59">
+        <v>0.14307489938509499</v>
+      </c>
+      <c r="E59">
+        <v>0.13825186956247301</v>
+      </c>
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>5.1257862978432399E-2</v>
+      </c>
+      <c r="D60">
+        <v>0.146543561700516</v>
+      </c>
+      <c r="E60">
+        <v>0.13826217062926599</v>
+      </c>
+      <c r="F60">
+        <v>7</v>
+      </c>
+      <c r="G60">
+        <v>100</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>4.3044064421081399E-2</v>
+      </c>
+      <c r="D61">
+        <v>0.14642241285365801</v>
+      </c>
+      <c r="E61">
+        <v>0.138568317520465</v>
+      </c>
+      <c r="F61">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>100</v>
+      </c>
+      <c r="H61">
+        <v>0.75</v>
+      </c>
+      <c r="I61">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <v>4.5893668401717803E-2</v>
+      </c>
+      <c r="D62">
+        <v>0.14629904187873</v>
+      </c>
+      <c r="E62">
+        <v>0.13870717837072399</v>
+      </c>
+      <c r="F62">
+        <v>8</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="H62">
+        <v>0.75</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <v>5.9441028632911203E-2</v>
+      </c>
+      <c r="D63">
+        <v>0.145177981217262</v>
+      </c>
+      <c r="E63">
+        <v>0.13879349299007199</v>
+      </c>
+      <c r="F63">
+        <v>6</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+      <c r="H63">
+        <v>0.75</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <v>6.2806992801472505E-2</v>
+      </c>
+      <c r="D64">
+        <v>0.143293972831186</v>
+      </c>
+      <c r="E64">
+        <v>0.13904527041735501</v>
+      </c>
+      <c r="F64">
+        <v>8</v>
+      </c>
+      <c r="G64">
+        <v>100</v>
+      </c>
+      <c r="H64">
+        <v>0.25</v>
+      </c>
+      <c r="I64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>5.8332861027077902E-2</v>
+      </c>
+      <c r="D65">
+        <v>0.14706090265218599</v>
+      </c>
+      <c r="E65">
+        <v>0.13913331192168299</v>
+      </c>
+      <c r="F65">
+        <v>6</v>
+      </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <v>4.8122379590069098E-2</v>
+      </c>
+      <c r="D66">
+        <v>0.145605956320915</v>
+      </c>
+      <c r="E66">
+        <v>0.13914193005440501</v>
+      </c>
+      <c r="F66">
+        <v>8</v>
+      </c>
+      <c r="G66">
+        <v>100</v>
+      </c>
+      <c r="H66">
+        <v>0.75</v>
+      </c>
+      <c r="I66">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <v>8.7746302049587693E-2</v>
+      </c>
+      <c r="D67">
+        <v>0.14244381918643301</v>
+      </c>
+      <c r="E67">
+        <v>0.13936924412111901</v>
+      </c>
+      <c r="F67">
+        <v>4</v>
+      </c>
+      <c r="G67">
+        <v>100</v>
+      </c>
+      <c r="H67">
+        <v>0.5</v>
+      </c>
+      <c r="I67">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <v>7.9838865244134902E-2</v>
+      </c>
+      <c r="D68">
+        <v>0.145453553914279</v>
+      </c>
+      <c r="E68">
+        <v>0.139700189841379</v>
+      </c>
+      <c r="F68">
+        <v>4</v>
+      </c>
+      <c r="G68">
+        <v>100</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <v>8.3765912352831096E-2</v>
+      </c>
+      <c r="D69">
+        <v>0.14343571889378401</v>
+      </c>
+      <c r="E69">
+        <v>0.13980990083832601</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69">
+        <v>100</v>
+      </c>
+      <c r="H69">
+        <v>0.5</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>5.63977178602144E-2</v>
+      </c>
+      <c r="D70">
+        <v>0.14403187566530701</v>
+      </c>
+      <c r="E70">
+        <v>0.13988558087141001</v>
+      </c>
+      <c r="F70">
+        <v>9</v>
+      </c>
+      <c r="G70">
+        <v>100</v>
+      </c>
+      <c r="H70">
+        <v>0.25</v>
+      </c>
+      <c r="I70">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <v>8.15777732379184E-2</v>
+      </c>
+      <c r="D71">
+        <v>0.14137956833779999</v>
+      </c>
+      <c r="E71">
+        <v>0.139959353927993</v>
+      </c>
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>100</v>
+      </c>
+      <c r="H71">
+        <v>0.25</v>
+      </c>
+      <c r="I71">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>6.8134556903949303E-2</v>
+      </c>
+      <c r="D72">
+        <v>0.145129361604284</v>
+      </c>
+      <c r="E72">
+        <v>0.14009931362187</v>
+      </c>
+      <c r="F72">
+        <v>5</v>
+      </c>
+      <c r="G72">
+        <v>100</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>6.8318372226432195E-2</v>
+      </c>
+      <c r="D73">
+        <v>0.14617629400648099</v>
+      </c>
+      <c r="E73">
+        <v>0.140348177421144</v>
+      </c>
+      <c r="F73">
+        <v>5</v>
+      </c>
+      <c r="G73">
+        <v>100</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>4.19622579655579E-2</v>
+      </c>
+      <c r="D74">
+        <v>0.146981226823442</v>
+      </c>
+      <c r="E74">
+        <v>0.14055257682900499</v>
+      </c>
+      <c r="F74">
+        <v>9</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+      <c r="H74">
+        <v>0.75</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>7.3025382276951004E-2</v>
+      </c>
+      <c r="D75">
+        <v>0.14345739328597601</v>
+      </c>
+      <c r="E75">
+        <v>0.14063979324048101</v>
+      </c>
+      <c r="F75">
+        <v>6</v>
+      </c>
+      <c r="G75">
+        <v>100</v>
+      </c>
+      <c r="H75">
+        <v>0.25</v>
+      </c>
+      <c r="I75">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <v>8.1514746657374404E-2</v>
+      </c>
+      <c r="D76">
+        <v>0.14485658189241701</v>
+      </c>
+      <c r="E76">
+        <v>0.14088654910901899</v>
+      </c>
+      <c r="F76">
+        <v>4</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <v>5.6067621030120203E-2</v>
+      </c>
+      <c r="D77">
+        <v>0.14484493413108401</v>
+      </c>
+      <c r="E77">
+        <v>0.14091135036338201</v>
+      </c>
+      <c r="F77">
+        <v>9</v>
+      </c>
+      <c r="G77">
+        <v>100</v>
+      </c>
+      <c r="H77">
+        <v>0.25</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <v>7.1275740851745706E-2</v>
+      </c>
+      <c r="D78">
+        <v>0.14401408629507401</v>
+      </c>
+      <c r="E78">
+        <v>0.141256863170997</v>
+      </c>
+      <c r="F78">
+        <v>6</v>
+      </c>
+      <c r="G78">
+        <v>100</v>
+      </c>
+      <c r="H78">
+        <v>0.25</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <v>6.5760570102767299E-2</v>
+      </c>
+      <c r="D79">
+        <v>0.143060929367681</v>
+      </c>
+      <c r="E79">
+        <v>0.14134189336223299</v>
+      </c>
+      <c r="F79">
+        <v>7</v>
+      </c>
+      <c r="G79">
+        <v>100</v>
+      </c>
+      <c r="H79">
+        <v>0.25</v>
+      </c>
+      <c r="I79">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="80" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <v>7.02121447880482E-2</v>
+      </c>
+      <c r="D80">
+        <v>0.14442869274334399</v>
+      </c>
+      <c r="E80">
+        <v>0.141626091158188</v>
+      </c>
+      <c r="F80">
+        <v>5</v>
+      </c>
+      <c r="G80">
+        <v>100</v>
+      </c>
+      <c r="H80">
+        <v>0.75</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <v>6.0947310334538499E-2</v>
+      </c>
+      <c r="D81">
+        <v>0.14281360048535499</v>
+      </c>
+      <c r="E81">
+        <v>0.14166281717534601</v>
+      </c>
+      <c r="F81">
+        <v>8</v>
+      </c>
+      <c r="G81">
+        <v>100</v>
+      </c>
+      <c r="H81">
+        <v>0.25</v>
+      </c>
+      <c r="I81">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C82">
+        <v>8.4573264748196805E-2</v>
+      </c>
+      <c r="D82">
+        <v>0.14263880365019199</v>
+      </c>
+      <c r="E82">
+        <v>0.141729831096984</v>
+      </c>
+      <c r="F82">
+        <v>4</v>
+      </c>
+      <c r="G82">
+        <v>100</v>
+      </c>
+      <c r="H82">
+        <v>0.5</v>
+      </c>
+      <c r="I82">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <v>0.10069861646385</v>
+      </c>
+      <c r="D83">
+        <v>0.144989364874194</v>
+      </c>
+      <c r="E83">
+        <v>0.14173722688958901</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>100</v>
+      </c>
+      <c r="H83">
+        <v>0.5</v>
+      </c>
+      <c r="I83">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <v>9.1460005635987898E-2</v>
+      </c>
+      <c r="D84">
+        <v>0.14341194997210599</v>
+      </c>
+      <c r="E84">
+        <v>0.14190782749721501</v>
+      </c>
+      <c r="F84">
+        <v>4</v>
+      </c>
+      <c r="G84">
+        <v>100</v>
+      </c>
+      <c r="H84">
+        <v>0.25</v>
+      </c>
+      <c r="I84">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <v>5.9729683637165298E-2</v>
+      </c>
+      <c r="D85">
+        <v>0.14442054676348001</v>
+      </c>
+      <c r="E85">
+        <v>0.14197785695262999</v>
+      </c>
+      <c r="F85">
+        <v>8</v>
+      </c>
+      <c r="G85">
+        <v>100</v>
+      </c>
+      <c r="H85">
+        <v>0.25</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C86">
+        <v>9.8613228343182702E-2</v>
+      </c>
+      <c r="D86">
+        <v>0.14529804730010401</v>
+      </c>
+      <c r="E86">
+        <v>0.14213958897658699</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>100</v>
+      </c>
+      <c r="H86">
+        <v>0.5</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C87">
+        <v>6.0499176068714203E-2</v>
+      </c>
+      <c r="D87">
+        <v>0.14376621811805201</v>
+      </c>
+      <c r="E87">
+        <v>0.14215368068834699</v>
+      </c>
+      <c r="F87">
+        <v>9</v>
+      </c>
+      <c r="G87">
+        <v>100</v>
+      </c>
+      <c r="H87">
+        <v>0.25</v>
+      </c>
+      <c r="I87">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C88">
+        <v>9.7581168165267296E-2</v>
+      </c>
+      <c r="D88">
+        <v>0.144858304599079</v>
+      </c>
+      <c r="E88">
+        <v>0.142428337238378</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>100</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C89">
+        <v>8.3622588057764499E-2</v>
+      </c>
+      <c r="D89">
+        <v>0.14226580071376799</v>
+      </c>
+      <c r="E89">
+        <v>0.14247461098046901</v>
+      </c>
+      <c r="F89">
+        <v>5</v>
+      </c>
+      <c r="G89">
+        <v>100</v>
+      </c>
+      <c r="H89">
+        <v>0.5</v>
+      </c>
+      <c r="I89">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C90">
+        <v>9.7445780083389402E-2</v>
+      </c>
+      <c r="D90">
+        <v>0.14554651511547301</v>
+      </c>
+      <c r="E90">
+        <v>0.14263470026584199</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>100</v>
+      </c>
+      <c r="H90">
+        <v>0.75</v>
+      </c>
+      <c r="I90">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="91" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C91">
+        <v>7.4014102873869003E-2</v>
+      </c>
+      <c r="D91">
+        <v>0.144121923512156</v>
+      </c>
+      <c r="E91">
+        <v>0.14295753154624699</v>
+      </c>
+      <c r="F91">
+        <v>8</v>
+      </c>
+      <c r="G91">
+        <v>100</v>
+      </c>
+      <c r="H91">
+        <v>0.25</v>
+      </c>
+      <c r="I91">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="92" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C92">
+        <v>7.9257992243272596E-2</v>
+      </c>
+      <c r="D92">
+        <v>0.14389390981997599</v>
+      </c>
+      <c r="E92">
+        <v>0.14302060787882101</v>
+      </c>
+      <c r="F92">
+        <v>5</v>
+      </c>
+      <c r="G92">
+        <v>100</v>
+      </c>
+      <c r="H92">
+        <v>0.25</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C93">
+        <v>9.5667087530106304E-2</v>
+      </c>
+      <c r="D93">
+        <v>0.14626256192692499</v>
+      </c>
+      <c r="E93">
+        <v>0.14322713571554499</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>100</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C94">
+        <v>0.10127236199049799</v>
+      </c>
+      <c r="D94">
+        <v>0.14460658880636101</v>
+      </c>
+      <c r="E94">
+        <v>0.143277019220173</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>100</v>
+      </c>
+      <c r="H94">
+        <v>0.75</v>
+      </c>
+      <c r="I94">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C95">
+        <v>6.5058478591712404E-2</v>
+      </c>
+      <c r="D95">
+        <v>0.14417569276692699</v>
+      </c>
+      <c r="E95">
+        <v>0.14331773105857901</v>
+      </c>
+      <c r="F95">
+        <v>7</v>
+      </c>
+      <c r="G95">
+        <v>100</v>
+      </c>
+      <c r="H95">
+        <v>0.25</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C96">
+        <v>9.3825548416289803E-2</v>
+      </c>
+      <c r="D96">
+        <v>0.143934840182634</v>
+      </c>
+      <c r="E96">
+        <v>0.14389828693981299</v>
+      </c>
+      <c r="F96">
+        <v>4</v>
+      </c>
+      <c r="G96">
+        <v>100</v>
+      </c>
+      <c r="H96">
+        <v>0.25</v>
+      </c>
+      <c r="I96">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C97">
+        <v>0.102535474397063</v>
+      </c>
+      <c r="D97">
+        <v>0.14509379898368799</v>
+      </c>
+      <c r="E97">
+        <v>0.14399571187065499</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>100</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="98" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C98">
+        <v>8.3919996534920493E-2</v>
+      </c>
+      <c r="D98">
+        <v>0.14316198088130599</v>
+      </c>
+      <c r="E98">
+        <v>0.14399663007628999</v>
+      </c>
+      <c r="F98">
+        <v>5</v>
+      </c>
+      <c r="G98">
+        <v>100</v>
+      </c>
+      <c r="H98">
+        <v>0.25</v>
+      </c>
+      <c r="I98">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C99">
+        <v>8.1801266304404305E-2</v>
+      </c>
+      <c r="D99">
+        <v>0.14368127160490601</v>
+      </c>
+      <c r="E99">
+        <v>0.14400039245664201</v>
+      </c>
+      <c r="F99">
+        <v>4</v>
+      </c>
+      <c r="G99">
+        <v>100</v>
+      </c>
+      <c r="H99">
+        <v>0.75</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C100">
+        <v>9.7545730496383196E-2</v>
+      </c>
+      <c r="D100">
+        <v>0.144623334216438</v>
+      </c>
+      <c r="E100">
+        <v>0.144053975744447</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>100</v>
+      </c>
+      <c r="H100">
+        <v>0.75</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C101">
+        <v>9.3617866360280799E-2</v>
+      </c>
+      <c r="D101">
+        <v>0.14321145223491599</v>
+      </c>
+      <c r="E101">
+        <v>0.14434358057525801</v>
+      </c>
+      <c r="F101">
+        <v>4</v>
+      </c>
+      <c r="G101">
+        <v>100</v>
+      </c>
+      <c r="H101">
+        <v>0.5</v>
+      </c>
+      <c r="I101">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="102" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C102">
+        <v>9.0821747314429505E-2</v>
+      </c>
+      <c r="D102">
+        <v>0.14407664942003701</v>
+      </c>
+      <c r="E102">
+        <v>0.14510244533772401</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+      <c r="G102">
+        <v>100</v>
+      </c>
+      <c r="H102">
+        <v>0.25</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C103">
+        <v>0.102244734953631</v>
+      </c>
+      <c r="D103">
+        <v>0.14418238953245799</v>
+      </c>
+      <c r="E103">
+        <v>0.14523454048312801</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+      <c r="G103">
+        <v>100</v>
+      </c>
+      <c r="H103">
+        <v>0.5</v>
+      </c>
+      <c r="I103">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C104">
+        <v>7.7009672770309304E-2</v>
+      </c>
+      <c r="D104">
+        <v>0.14488874152161499</v>
+      </c>
+      <c r="E104">
+        <v>0.14535498880393499</v>
+      </c>
+      <c r="F104">
+        <v>7</v>
+      </c>
+      <c r="G104">
+        <v>100</v>
+      </c>
+      <c r="H104">
+        <v>0.25</v>
+      </c>
+      <c r="I104">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="105" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C105">
+        <v>9.3463797509620805E-2</v>
+      </c>
+      <c r="D105">
+        <v>0.14560307985315299</v>
+      </c>
+      <c r="E105">
+        <v>0.14541301841867599</v>
+      </c>
+      <c r="F105">
+        <v>5</v>
+      </c>
+      <c r="G105">
+        <v>100</v>
+      </c>
+      <c r="H105">
+        <v>0.25</v>
+      </c>
+      <c r="I105">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C106">
+        <v>6.9744113181652606E-2</v>
+      </c>
+      <c r="D106">
+        <v>0.14486636258719299</v>
+      </c>
+      <c r="E106">
+        <v>0.14582533097598499</v>
+      </c>
+      <c r="F106">
+        <v>9</v>
+      </c>
+      <c r="G106">
+        <v>100</v>
+      </c>
+      <c r="H106">
+        <v>0.25</v>
+      </c>
+      <c r="I106">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="107" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C107">
+        <v>0.10303396651225601</v>
+      </c>
+      <c r="D107">
+        <v>0.14521334146645801</v>
+      </c>
+      <c r="E107">
+        <v>0.14602015656395101</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>100</v>
+      </c>
+      <c r="H107">
+        <v>0.75</v>
+      </c>
+      <c r="I107">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C108">
+        <v>9.6891455759104197E-2</v>
+      </c>
+      <c r="D108">
+        <v>0.145744622303416</v>
+      </c>
+      <c r="E108">
+        <v>0.146253459573707</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108">
+        <v>100</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="109" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C109">
+        <v>8.4342159326828203E-2</v>
+      </c>
+      <c r="D109">
+        <v>0.144608928777331</v>
+      </c>
+      <c r="E109">
+        <v>0.146845883088326</v>
+      </c>
+      <c r="F109">
+        <v>6</v>
+      </c>
+      <c r="G109">
+        <v>100</v>
+      </c>
+      <c r="H109">
+        <v>0.25</v>
+      </c>
+      <c r="I109">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C110">
+        <v>0.106409157773387</v>
+      </c>
+      <c r="D110">
+        <v>0.14625226837623401</v>
+      </c>
+      <c r="E110">
+        <v>0.14688061224138299</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>100</v>
+      </c>
+      <c r="H110">
+        <v>0.5</v>
+      </c>
+      <c r="I110">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="111" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C111">
+        <v>0.10672788557386099</v>
+      </c>
+      <c r="D111">
+        <v>0.145701393121353</v>
+      </c>
+      <c r="E111">
+        <v>0.14755954260977</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+      <c r="G111">
+        <v>100</v>
+      </c>
+      <c r="H111">
+        <v>0.25</v>
+      </c>
+      <c r="I111">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C112">
+        <v>0.104919609523874</v>
+      </c>
+      <c r="D112">
+        <v>0.14665893062836799</v>
+      </c>
+      <c r="E112">
+        <v>0.14765263961917999</v>
+      </c>
+      <c r="F112">
+        <v>3</v>
+      </c>
+      <c r="G112">
+        <v>100</v>
+      </c>
+      <c r="H112">
+        <v>0.25</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C113">
+        <v>0.107888802210363</v>
+      </c>
+      <c r="D113">
+        <v>0.14656832233735501</v>
+      </c>
+      <c r="E113">
+        <v>0.15048967996853399</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+      <c r="G113">
+        <v>100</v>
+      </c>
+      <c r="H113">
+        <v>0.25</v>
+      </c>
+      <c r="I113">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C114">
+        <v>0.10235675824731499</v>
+      </c>
+      <c r="D114">
+        <v>0.14656887131308499</v>
+      </c>
+      <c r="E114">
+        <v>0.151297413732012</v>
+      </c>
+      <c r="F114">
+        <v>4</v>
+      </c>
+      <c r="G114">
+        <v>100</v>
+      </c>
+      <c r="H114">
+        <v>0.25</v>
+      </c>
+      <c r="I114">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C115">
+        <v>0.11646354126544101</v>
+      </c>
+      <c r="D115">
+        <v>0.14985155299558001</v>
+      </c>
+      <c r="E115">
+        <v>0.15700533998136601</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <v>100</v>
+      </c>
+      <c r="H115">
+        <v>0.25</v>
+      </c>
+      <c r="I115">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="C6:I115">
+    <sortCondition ref="E5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>